<commit_message>
Change import 1 to multiple files
</commit_message>
<xml_diff>
--- a/input_import.xlsx
+++ b/input_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d18a68728dcd25ae/__Study/Python/Side Projects/Push-files-to-SQL-Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{B1395638-CDA4-4C9F-8F60-B83171E2FEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05DEC0ED-A538-465D-A0D1-083BBEC322F2}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:40009_{B1395638-CDA4-4C9F-8F60-B83171E2FEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7318B77F-C6BB-40AF-B2A2-E233AF63CBD4}"/>
   <bookViews>
-    <workbookView xWindow="21255" yWindow="2100" windowWidth="28350" windowHeight="16785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21255" yWindow="2100" windowWidth="28350" windowHeight="16785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list_folders_to_import_db" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>directory</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>table_name</t>
   </si>
 </sst>
 </file>
@@ -899,43 +899,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -947,32 +947,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>